<commit_message>
[Update] example 005 업데이트
</commit_message>
<xml_diff>
--- a/example/005.Database/Meta/Item.xlsx
+++ b/example/005.Database/Meta/Item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>ITEM_ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -162,6 +162,22 @@
   </si>
   <si>
     <t>ItemName030</t>
+  </si>
+  <si>
+    <t>STAT.STAT_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STAT.VALUE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FLOAT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -510,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -524,9 +540,10 @@
     <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -545,8 +562,14 @@
       <c r="F1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -565,8 +588,14 @@
       <c r="F2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>100001</v>
       </c>
@@ -585,8 +614,14 @@
       <c r="F3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>100002</v>
       </c>
@@ -605,8 +640,14 @@
       <c r="F4">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>100003</v>
       </c>
@@ -625,8 +666,14 @@
       <c r="F5">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>100004</v>
       </c>
@@ -645,8 +692,14 @@
       <c r="F6">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>100005</v>
       </c>
@@ -665,8 +718,14 @@
       <c r="F7">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>100006</v>
       </c>
@@ -685,8 +744,14 @@
       <c r="F8">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>100007</v>
       </c>
@@ -705,8 +770,14 @@
       <c r="F9">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>100008</v>
       </c>
@@ -725,8 +796,14 @@
       <c r="F10">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>100009</v>
       </c>
@@ -745,8 +822,14 @@
       <c r="F11">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>100010</v>
       </c>
@@ -765,8 +848,14 @@
       <c r="F12">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>100011</v>
       </c>
@@ -785,8 +874,14 @@
       <c r="F13">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>100012</v>
       </c>
@@ -805,8 +900,14 @@
       <c r="F14">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>100013</v>
       </c>
@@ -825,8 +926,14 @@
       <c r="F15">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>100014</v>
       </c>
@@ -845,8 +952,14 @@
       <c r="F16">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>100015</v>
       </c>
@@ -865,8 +978,14 @@
       <c r="F17">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>100016</v>
       </c>
@@ -885,8 +1004,14 @@
       <c r="F18">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>100017</v>
       </c>
@@ -905,8 +1030,14 @@
       <c r="F19">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>100018</v>
       </c>
@@ -925,8 +1056,14 @@
       <c r="F20">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>100019</v>
       </c>
@@ -945,8 +1082,14 @@
       <c r="F21">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>100020</v>
       </c>
@@ -965,8 +1108,14 @@
       <c r="F22">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>100021</v>
       </c>
@@ -985,8 +1134,14 @@
       <c r="F23">
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>100022</v>
       </c>
@@ -1005,8 +1160,14 @@
       <c r="F24">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>100023</v>
       </c>
@@ -1025,8 +1186,14 @@
       <c r="F25">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>100024</v>
       </c>
@@ -1045,8 +1212,14 @@
       <c r="F26">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>100025</v>
       </c>
@@ -1065,8 +1238,14 @@
       <c r="F27">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>100026</v>
       </c>
@@ -1085,8 +1264,14 @@
       <c r="F28">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>100027</v>
       </c>
@@ -1105,8 +1290,14 @@
       <c r="F29">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>100028</v>
       </c>
@@ -1125,8 +1316,14 @@
       <c r="F30">
         <v>100</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>100029</v>
       </c>
@@ -1145,8 +1342,14 @@
       <c r="F31">
         <v>100</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>100030</v>
       </c>
@@ -1164,6 +1367,12 @@
       </c>
       <c r="F32">
         <v>100</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>